<commit_message>
Update testdata files with latest configuration changes and remove temporary files
- Update DBRT_Config.json with new multileader style and note block configuration
- Update ProjectConfig.json with additional multileader styles and note block settings
- Clean up temporary AutoCAD lock files (.dwl, .dwl2) and error logs
- Update drawing files with latest changes from testing

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/testdata/DBRT Test/DBRT_Index.xlsx
+++ b/testdata/DBRT Test/DBRT_Index.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevorp\Dev\KPFF.AutoCAD.DraftingAssistant\testdata\DBRT Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C011539B-F8BE-4C91-9482-AB7A86D3844A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B72384-FFB7-428D-BE84-016F8AE35ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
-    <sheet name="ABC Notes" sheetId="2" r:id="rId2"/>
-    <sheet name="DEF Notes" sheetId="5" r:id="rId3"/>
+    <sheet name="PV Notes" sheetId="2" r:id="rId2"/>
+    <sheet name="SP Notes" sheetId="5" r:id="rId3"/>
     <sheet name="Excel Notes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="60">
   <si>
     <t>Sheet</t>
   </si>
@@ -126,12 +125,6 @@
     <t>Note 24</t>
   </si>
   <si>
-    <t>ABC-101</t>
-  </si>
-  <si>
-    <t>ABC-102</t>
-  </si>
-  <si>
     <t>File</t>
   </si>
   <si>
@@ -141,24 +134,12 @@
     <t>CONSTRUCT SIDEWALK</t>
   </si>
   <si>
-    <t>ABC-103</t>
-  </si>
-  <si>
     <t>CONSTRUCT ROADWAY</t>
   </si>
   <si>
     <t>CONSTRUCT UTILITY</t>
   </si>
   <si>
-    <t>DEF-101</t>
-  </si>
-  <si>
-    <t>DEF-102</t>
-  </si>
-  <si>
-    <t>DEF-103</t>
-  </si>
-  <si>
     <t>Designed By</t>
   </si>
   <si>
@@ -210,9 +191,6 @@
     <t>PV-204A</t>
   </si>
   <si>
-    <t>STATION/LOCATION</t>
-  </si>
-  <si>
     <t>PAVING PLAN</t>
   </si>
   <si>
@@ -234,13 +212,13 @@
     <t>Checked Date</t>
   </si>
   <si>
-    <t>XX/XXXX</t>
-  </si>
-  <si>
     <t>Sheet Number</t>
   </si>
   <si>
-    <t>XXX</t>
+    <t>08/2025</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -262,18 +240,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor theme="0" tint="-0.14999847407452621"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -290,22 +262,14 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <font>
         <b val="0"/>
@@ -323,30 +287,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -357,7 +307,6 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -389,13 +338,7 @@
       </font>
       <fill>
         <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -417,6 +360,79 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -432,28 +448,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A4F1CBB4-2842-41F7-ABFB-5882B559A8DC}" name="SHEET_INDEX" displayName="SHEET_INDEX" ref="A1:L6" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A4F1CBB4-2842-41F7-ABFB-5882B559A8DC}" name="SHEET_INDEX" displayName="SHEET_INDEX" ref="A1:L6" totalsRowShown="0" dataDxfId="2">
   <autoFilter ref="A1:L6" xr:uid="{A4F1CBB4-2842-41F7-ABFB-5882B559A8DC}"/>
   <tableColumns count="12">
-    <tableColumn id="3" xr3:uid="{3F2713EA-FF09-4ABE-994F-102E702E9565}" name="File"/>
-    <tableColumn id="4" xr3:uid="{491846AA-90A1-489B-8390-792C5C135E7F}" name="Sheet"/>
-    <tableColumn id="10" xr3:uid="{E242E832-64A3-463A-B2C4-25A759ABBF89}" name="Submittal"/>
-    <tableColumn id="9" xr3:uid="{CD1252F7-879C-43D0-B741-BB821959577C}" name="Title"/>
-    <tableColumn id="1" xr3:uid="{A6197A5E-891A-48C8-A378-8A1248F021F2}" name="Subtitle" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{86BB227D-4F71-401E-8A46-55DD2809D1EC}" name="Sheet Number" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{0E4A50F3-5C36-48E6-8740-12D9CE401BBB}" name="Designed By" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{4DB85713-0457-4BE5-A410-FCE80123A20C}" name="Checked By" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{E5E36AF6-F67D-4B8D-997A-B74EBA5B6B71}" name="Approved By" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{135B9ECD-3A42-423B-B667-D4CE7C1C5CE0}" name="Designed Date" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{69BDD4E0-DB04-4E42-BC04-7BD8BBF4BCF1}" name="Checked Date" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{7D9F4D45-F4B8-4C0D-89A0-4798DCC0F56C}" name="Approved Date" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{3F2713EA-FF09-4ABE-994F-102E702E9565}" name="File" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{491846AA-90A1-489B-8390-792C5C135E7F}" name="Sheet" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{E242E832-64A3-463A-B2C4-25A759ABBF89}" name="Submittal" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{CD1252F7-879C-43D0-B741-BB821959577C}" name="Title" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{A6197A5E-891A-48C8-A378-8A1248F021F2}" name="Subtitle" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{86BB227D-4F71-401E-8A46-55DD2809D1EC}" name="Sheet Number" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{0E4A50F3-5C36-48E6-8740-12D9CE401BBB}" name="Designed By" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{4DB85713-0457-4BE5-A410-FCE80123A20C}" name="Checked By" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{E5E36AF6-F67D-4B8D-997A-B74EBA5B6B71}" name="Approved By" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{135B9ECD-3A42-423B-B667-D4CE7C1C5CE0}" name="Designed Date" dataDxfId="3">
+      <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{69BDD4E0-DB04-4E42-BC04-7BD8BBF4BCF1}" name="Checked Date" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{7D9F4D45-F4B8-4C0D-89A0-4798DCC0F56C}" name="Approved Date" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}" name="ABC_NOTES" displayName="ABC_NOTES" ref="A1:B6" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}" name="PV_NOTES" displayName="PV_NOTES" ref="A1:B6" totalsRowShown="0">
   <autoFilter ref="A1:B6" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1DFF5014-936E-44DB-A95A-177B5B5D0D2C}" name="Number"/>
@@ -464,7 +482,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A184BDBD-A5F9-44CB-A083-C6BD71A9816B}" name="DEF_NOTES" displayName="DEF_NOTES" ref="A1:B6" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A184BDBD-A5F9-44CB-A083-C6BD71A9816B}" name="SP_NOTES" displayName="SP_NOTES" ref="A1:B6" totalsRowShown="0">
   <autoFilter ref="A1:B6" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{05061837-533E-4FDE-B2B4-0C0FEBE640B0}" name="Number"/>
@@ -475,8 +493,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C167B881-E5F9-44DB-8BC8-EC4D2F202D87}" name="EXCEL_NOTES" displayName="EXCEL_NOTES" ref="A1:Y7" totalsRowShown="0">
-  <autoFilter ref="A1:Y7" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C167B881-E5F9-44DB-8BC8-EC4D2F202D87}" name="EXCEL_NOTES" displayName="EXCEL_NOTES" ref="A1:Y6" totalsRowShown="0">
+  <autoFilter ref="A1:Y6" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -854,7 +872,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,239 +888,237 @@
     <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.88671875" customWidth="1"/>
-    <col min="16" max="18" width="15.77734375" customWidth="1"/>
+    <col min="12" max="13" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.88671875" customWidth="1"/>
+    <col min="15" max="17" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" t="s">
-        <v>61</v>
-      </c>
-      <c r="K1" t="s">
-        <v>63</v>
-      </c>
-      <c r="L1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="K2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="E4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="D6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>44</v>
+      <c r="E6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1139,7 +1155,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1147,7 +1163,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1155,7 +1171,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1163,7 +1179,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1171,7 +1187,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1187,7 +1203,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1209,7 +1225,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1217,7 +1233,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1225,7 +1241,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1233,7 +1249,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1241,7 +1257,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1254,10 +1270,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF1246F-34C5-4C20-93A7-4C83B8F18203}">
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1344,7 +1360,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -1352,7 +1368,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -1360,7 +1376,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -1368,7 +1384,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -1376,17 +1392,9 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update SHEET_INDEX table description for clarity
- Changed "List of all sheets and metadata, including containing file name and title block attributes"
- To "List of all sheets including DWG file name and title block attributes"
- Previous commits included major UI improvements:
  * Removed Enable Plotting checkbox and Plot Format Settings
  * Updated folder selection dialogs with modern approach
  * Fixed sheet counting and configuration display
  * Updated label texts for Title Blocks and Construction Notes tabs

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/testdata/DBRT Test/DBRT_Index.xlsx
+++ b/testdata/DBRT Test/DBRT_Index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevorp\Dev\KPFF.AutoCAD.DraftingAssistant\testdata\DBRT Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B72384-FFB7-428D-BE84-016F8AE35ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6FCE99-6F7B-4682-9880-525C1D07A690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="59">
   <si>
     <t>Sheet</t>
   </si>
@@ -128,18 +128,6 @@
     <t>File</t>
   </si>
   <si>
-    <t>CONSTRUCT CURB</t>
-  </si>
-  <si>
-    <t>CONSTRUCT SIDEWALK</t>
-  </si>
-  <si>
-    <t>CONSTRUCT ROADWAY</t>
-  </si>
-  <si>
-    <t>CONSTRUCT UTILITY</t>
-  </si>
-  <si>
     <t>Designed By</t>
   </si>
   <si>
@@ -152,73 +140,82 @@
     <t>TMP</t>
   </si>
   <si>
+    <t>DBRT-PV2</t>
+  </si>
+  <si>
+    <t>PV-201</t>
+  </si>
+  <si>
+    <t>PV-202</t>
+  </si>
+  <si>
+    <t>PV-203</t>
+  </si>
+  <si>
+    <t>PV-204</t>
+  </si>
+  <si>
+    <t>PV-204A</t>
+  </si>
+  <si>
+    <t>Subtitle</t>
+  </si>
+  <si>
+    <t>Submittal</t>
+  </si>
+  <si>
+    <t>30% SUBMITTAL</t>
+  </si>
+  <si>
+    <t>Designed Date</t>
+  </si>
+  <si>
+    <t>Approved Date</t>
+  </si>
+  <si>
+    <t>Checked Date</t>
+  </si>
+  <si>
+    <t>Sheet Number</t>
+  </si>
+  <si>
+    <t>09/2025</t>
+  </si>
+  <si>
     <t>ALP</t>
   </si>
   <si>
     <t>CBP</t>
   </si>
   <si>
-    <t>FROM EXCEL</t>
-  </si>
-  <si>
-    <t>CONSTRUCT</t>
-  </si>
-  <si>
-    <t>INSTALL</t>
-  </si>
-  <si>
-    <t>PROTECT</t>
-  </si>
-  <si>
-    <t>ADJUST</t>
-  </si>
-  <si>
-    <t>DBRT-PV2</t>
-  </si>
-  <si>
-    <t>PV-201</t>
-  </si>
-  <si>
-    <t>PV-202</t>
-  </si>
-  <si>
-    <t>PV-203</t>
-  </si>
-  <si>
-    <t>PV-204</t>
-  </si>
-  <si>
-    <t>PV-204A</t>
-  </si>
-  <si>
-    <t>PAVING PLAN</t>
-  </si>
-  <si>
-    <t>Subtitle</t>
-  </si>
-  <si>
-    <t>Submittal</t>
-  </si>
-  <si>
-    <t>30% SUBMITTAL</t>
-  </si>
-  <si>
-    <t>Designed Date</t>
-  </si>
-  <si>
-    <t>Approved Date</t>
-  </si>
-  <si>
-    <t>Checked Date</t>
-  </si>
-  <si>
-    <t>Sheet Number</t>
-  </si>
-  <si>
-    <t>08/2025</t>
-  </si>
-  <si>
-    <t>TEST</t>
+    <t>DBRT-SP2</t>
+  </si>
+  <si>
+    <t>SP-201</t>
+  </si>
+  <si>
+    <t>SP-202</t>
+  </si>
+  <si>
+    <t>SP-203</t>
+  </si>
+  <si>
+    <t>SP-204</t>
+  </si>
+  <si>
+    <t>SP-204A</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+  </si>
+  <si>
+    <t>SUBTITLE</t>
+  </si>
+  <si>
+    <t>PV NOTE</t>
+  </si>
+  <si>
+    <t>SP NOTE</t>
   </si>
 </sst>
 </file>
@@ -260,11 +257,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -301,13 +296,6 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -434,6 +422,13 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -448,19 +443,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A4F1CBB4-2842-41F7-ABFB-5882B559A8DC}" name="SHEET_INDEX" displayName="SHEET_INDEX" ref="A1:L6" totalsRowShown="0" dataDxfId="2">
-  <autoFilter ref="A1:L6" xr:uid="{A4F1CBB4-2842-41F7-ABFB-5882B559A8DC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A4F1CBB4-2842-41F7-ABFB-5882B559A8DC}" name="SHEET_INDEX" displayName="SHEET_INDEX" ref="A1:L11" totalsRowShown="0" dataDxfId="12">
+  <autoFilter ref="A1:L11" xr:uid="{A4F1CBB4-2842-41F7-ABFB-5882B559A8DC}"/>
   <tableColumns count="12">
-    <tableColumn id="3" xr3:uid="{3F2713EA-FF09-4ABE-994F-102E702E9565}" name="File" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{491846AA-90A1-489B-8390-792C5C135E7F}" name="Sheet" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{E242E832-64A3-463A-B2C4-25A759ABBF89}" name="Submittal" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{CD1252F7-879C-43D0-B741-BB821959577C}" name="Title" dataDxfId="9"/>
-    <tableColumn id="1" xr3:uid="{A6197A5E-891A-48C8-A378-8A1248F021F2}" name="Subtitle" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{86BB227D-4F71-401E-8A46-55DD2809D1EC}" name="Sheet Number" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{0E4A50F3-5C36-48E6-8740-12D9CE401BBB}" name="Designed By" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{4DB85713-0457-4BE5-A410-FCE80123A20C}" name="Checked By" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{E5E36AF6-F67D-4B8D-997A-B74EBA5B6B71}" name="Approved By" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{135B9ECD-3A42-423B-B667-D4CE7C1C5CE0}" name="Designed Date" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{3F2713EA-FF09-4ABE-994F-102E702E9565}" name="File" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{491846AA-90A1-489B-8390-792C5C135E7F}" name="Sheet" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{E242E832-64A3-463A-B2C4-25A759ABBF89}" name="Submittal" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{CD1252F7-879C-43D0-B741-BB821959577C}" name="Title" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{A6197A5E-891A-48C8-A378-8A1248F021F2}" name="Subtitle" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{86BB227D-4F71-401E-8A46-55DD2809D1EC}" name="Sheet Number" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{0E4A50F3-5C36-48E6-8740-12D9CE401BBB}" name="Designed By" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{4DB85713-0457-4BE5-A410-FCE80123A20C}" name="Checked By" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{E5E36AF6-F67D-4B8D-997A-B74EBA5B6B71}" name="Approved By" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{135B9ECD-3A42-423B-B667-D4CE7C1C5CE0}" name="Designed Date" dataDxfId="2">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{69BDD4E0-DB04-4E42-BC04-7BD8BBF4BCF1}" name="Checked Date" dataDxfId="1"/>
@@ -493,8 +488,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C167B881-E5F9-44DB-8BC8-EC4D2F202D87}" name="EXCEL_NOTES" displayName="EXCEL_NOTES" ref="A1:Y6" totalsRowShown="0">
-  <autoFilter ref="A1:Y6" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C167B881-E5F9-44DB-8BC8-EC4D2F202D87}" name="EXCEL_NOTES" displayName="EXCEL_NOTES" ref="A1:Y11" totalsRowShown="0">
+  <autoFilter ref="A1:Y11" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -869,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A56E6E1-F0E6-45B8-A4FD-BDCEFA26A2B5}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -880,7 +875,7 @@
     <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
@@ -901,224 +896,414 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
         <v>51</v>
       </c>
-      <c r="F1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
         <v>54</v>
       </c>
-      <c r="K1" t="s">
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" t="s">
         <v>56</v>
       </c>
-      <c r="L1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="2">
-        <v>2</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="2">
-        <v>3</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="H11" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" s="2">
-        <v>4</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="2">
-        <v>5</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>58</v>
+      <c r="I11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1134,7 +1319,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A58DC59-E790-4B42-8F44-52FF796EA0AA}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1155,7 +1342,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1163,7 +1350,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1171,7 +1358,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1179,7 +1366,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1187,10 +1374,11 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1202,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE7284E-F66F-4B31-BB75-3E5641C2CCDF}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1225,7 +1413,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1233,7 +1421,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1241,7 +1429,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1249,7 +1437,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1257,7 +1445,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1270,10 +1458,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF1246F-34C5-4C20-93A7-4C83B8F18203}">
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1360,7 +1548,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -1368,7 +1556,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -1376,7 +1564,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -1384,7 +1572,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -1392,9 +1580,49 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11">
         <v>5</v>
       </c>
     </row>

</xml_diff>